<commit_message>
impedir que um apartamento tenha mais de 2 vagas
</commit_message>
<xml_diff>
--- a/templateExcel/modelo_vagas_sorteio.xlsx
+++ b/templateExcel/modelo_vagas_sorteio.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcs-r\OneDrive\Área de Trabalho\Vagas - condominio\Regras\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\SorteioVagasCondominio\templateExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D7F081-93A4-4D1F-A30E-1425E3A68C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDF7412-E1E8-44DF-9A87-684C2BF713D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vagas" sheetId="1" r:id="rId1"/>
@@ -502,7 +502,7 @@
   <dimension ref="A1:E129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -584,7 +584,10 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -598,7 +601,10 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -612,7 +618,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>2002</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -654,7 +663,10 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1232,7 +1244,10 @@
         <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E47">
+        <v>203</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1246,7 +1261,10 @@
         <v>8</v>
       </c>
       <c r="D48" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E48">
+        <v>204</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1333,7 +1351,10 @@
         <v>8</v>
       </c>
       <c r="D54" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E54">
+        <v>205</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1347,7 +1368,10 @@
         <v>8</v>
       </c>
       <c r="D55" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E55">
+        <v>1101</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1909,7 +1933,10 @@
         <v>8</v>
       </c>
       <c r="D93" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E93">
+        <v>206</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -1937,7 +1964,10 @@
         <v>8</v>
       </c>
       <c r="D95" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E95">
+        <v>2003</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -1951,7 +1981,10 @@
         <v>8</v>
       </c>
       <c r="D96" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E96">
+        <v>2003</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2021,7 +2054,10 @@
         <v>8</v>
       </c>
       <c r="D101" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E101">
+        <v>306</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>